<commit_message>
adding significant age code to imputed running manova
</commit_message>
<xml_diff>
--- a/age_est_data1.xlsx
+++ b/age_est_data1.xlsx
@@ -406,20 +406,20 @@
         </is>
       </c>
       <c r="B2">
-        <v>-2.204</v>
+        <v>-2.023</v>
       </c>
       <c r="C2">
-        <v>0.263</v>
+        <v>0.239</v>
       </c>
       <c r="D2">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E2">
-        <v>-8.382999999999999</v>
+        <v>-8.458</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.6358e-12</t>
+          <t>4.6513e-11</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -440,20 +440,20 @@
         </is>
       </c>
       <c r="B3">
-        <v>-3.228</v>
+        <v>-3.012</v>
       </c>
       <c r="C3">
-        <v>0.636</v>
+        <v>0.595</v>
       </c>
       <c r="D3">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E3">
-        <v>-5.075</v>
+        <v>-5.067</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.2876e-06</t>
+          <t>1.3204e-06</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -474,20 +474,20 @@
         </is>
       </c>
       <c r="B4">
-        <v>-1.024</v>
+        <v>-0.989</v>
       </c>
       <c r="C4">
-        <v>0.638</v>
+        <v>0.597</v>
       </c>
       <c r="D4">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E4">
-        <v>-1.605</v>
+        <v>-1.658</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2.4387e-01</t>
+          <t>2.2174e-01</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -508,20 +508,20 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.651</v>
+        <v>0.444</v>
       </c>
       <c r="C5">
-        <v>0.463</v>
+        <v>0.42</v>
       </c>
       <c r="D5">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E5">
-        <v>1.405</v>
+        <v>1.058</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>3.3859e-01</t>
+          <t>5.4041e-01</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -542,20 +542,20 @@
         </is>
       </c>
       <c r="B6">
-        <v>2.752</v>
+        <v>2.886</v>
       </c>
       <c r="C6">
-        <v>1.121</v>
+        <v>1.044</v>
       </c>
       <c r="D6">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E6">
-        <v>2.455</v>
+        <v>2.764</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3.7701e-02</t>
+          <t>1.5873e-02</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -576,20 +576,20 @@
         </is>
       </c>
       <c r="B7">
-        <v>2.101</v>
+        <v>2.442</v>
       </c>
       <c r="C7">
-        <v>1.125</v>
+        <v>1.048</v>
       </c>
       <c r="D7">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E7">
-        <v>1.868</v>
+        <v>2.331</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1.4830e-01</t>
+          <t>5.1904e-02</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -610,20 +610,20 @@
         </is>
       </c>
       <c r="B8">
-        <v>-7.709</v>
+        <v>-7.036</v>
       </c>
       <c r="C8">
-        <v>0.643</v>
+        <v>0.585</v>
       </c>
       <c r="D8">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E8">
-        <v>-11.991</v>
+        <v>-12.019</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1.6044e-12</t>
+          <t>4.6484e-11</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -644,20 +644,20 @@
         </is>
       </c>
       <c r="B9">
-        <v>-10.191</v>
+        <v>-8.795</v>
       </c>
       <c r="C9">
-        <v>1.555</v>
+        <v>1.455</v>
       </c>
       <c r="D9">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E9">
-        <v>-6.552</v>
+        <v>-6.044</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2.2804e-10</t>
+          <t>5.3946e-09</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -678,20 +678,20 @@
         </is>
       </c>
       <c r="B10">
-        <v>-2.482</v>
+        <v>-1.759</v>
       </c>
       <c r="C10">
-        <v>1.561</v>
+        <v>1.46</v>
       </c>
       <c r="D10">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E10">
-        <v>-1.59</v>
+        <v>-1.205</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2.5018e-01</t>
+          <t>4.5053e-01</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -712,20 +712,20 @@
         </is>
       </c>
       <c r="B11">
-        <v>-0.945</v>
+        <v>-0.862</v>
       </c>
       <c r="C11">
-        <v>0.119</v>
+        <v>0.107</v>
       </c>
       <c r="D11">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E11">
-        <v>-7.969</v>
+        <v>-8.042999999999999</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1.6505e-12</t>
+          <t>4.6526e-11</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -746,20 +746,20 @@
         </is>
       </c>
       <c r="B12">
-        <v>-1.01</v>
+        <v>-1.014</v>
       </c>
       <c r="C12">
-        <v>0.287</v>
+        <v>0.266</v>
       </c>
       <c r="D12">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E12">
-        <v>-3.521</v>
+        <v>-3.806</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>1.2805e-03</t>
+          <t>4.2653e-04</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -780,20 +780,20 @@
         </is>
       </c>
       <c r="B13">
-        <v>-0.065</v>
+        <v>-0.152</v>
       </c>
       <c r="C13">
-        <v>0.288</v>
+        <v>0.267</v>
       </c>
       <c r="D13">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E13">
-        <v>-0.227</v>
+        <v>-0.5679999999999999</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>9.7203e-01</t>
+          <t>8.3691e-01</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -814,20 +814,20 @@
         </is>
       </c>
       <c r="B14">
-        <v>-0.589</v>
+        <v>-0.6860000000000001</v>
       </c>
       <c r="C14">
-        <v>0.192</v>
+        <v>0.175</v>
       </c>
       <c r="D14">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E14">
-        <v>-3.073</v>
+        <v>-3.925</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>6.1003e-03</t>
+          <t>2.6383e-04</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -848,20 +848,20 @@
         </is>
       </c>
       <c r="B15">
-        <v>-0.725</v>
+        <v>-0.819</v>
       </c>
       <c r="C15">
-        <v>0.464</v>
+        <v>0.434</v>
       </c>
       <c r="D15">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E15">
-        <v>-1.563</v>
+        <v>-1.887</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2.6189e-01</t>
+          <t>1.4276e-01</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -882,20 +882,20 @@
         </is>
       </c>
       <c r="B16">
-        <v>-0.136</v>
+        <v>-0.133</v>
       </c>
       <c r="C16">
-        <v>0.465</v>
+        <v>0.436</v>
       </c>
       <c r="D16">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E16">
-        <v>-0.292</v>
+        <v>-0.306</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>9.5398e-01</t>
+          <t>9.4957e-01</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -916,20 +916,20 @@
         </is>
       </c>
       <c r="B17">
-        <v>-1.251</v>
+        <v>-1.363</v>
       </c>
       <c r="C17">
-        <v>0.417</v>
+        <v>0.369</v>
       </c>
       <c r="D17">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E17">
-        <v>-2.997</v>
+        <v>-3.699</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>7.7968e-03</t>
+          <t>6.5142e-04</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -950,20 +950,20 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.742</v>
+        <v>0.762</v>
       </c>
       <c r="C18">
-        <v>1.01</v>
+        <v>0.916</v>
       </c>
       <c r="D18">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E18">
-        <v>0.735</v>
+        <v>0.832</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>7.4299e-01</t>
+          <t>6.8304e-01</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -984,20 +984,20 @@
         </is>
       </c>
       <c r="B19">
-        <v>1.993</v>
+        <v>2.126</v>
       </c>
       <c r="C19">
-        <v>1.013</v>
+        <v>0.919</v>
       </c>
       <c r="D19">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E19">
-        <v>1.966</v>
+        <v>2.312</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>1.2090e-01</t>
+          <t>5.4340e-02</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1018,20 +1018,20 @@
         </is>
       </c>
       <c r="B20">
-        <v>-6.483</v>
+        <v>-6.213</v>
       </c>
       <c r="C20">
-        <v>0.555</v>
+        <v>0.513</v>
       </c>
       <c r="D20">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E20">
-        <v>-11.673</v>
+        <v>-12.106</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>1.6046e-12</t>
+          <t>4.6484e-11</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1052,20 +1052,20 @@
         </is>
       </c>
       <c r="B21">
-        <v>-7.966</v>
+        <v>-7.079</v>
       </c>
       <c r="C21">
-        <v>1.344</v>
+        <v>1.276</v>
       </c>
       <c r="D21">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E21">
-        <v>-5.929</v>
+        <v>-5.549</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>1.1100e-08</t>
+          <t>9.7485e-08</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1086,20 +1086,20 @@
         </is>
       </c>
       <c r="B22">
-        <v>-1.483</v>
+        <v>-0.865</v>
       </c>
       <c r="C22">
-        <v>1.348</v>
+        <v>1.28</v>
       </c>
       <c r="D22">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E22">
-        <v>-1.1</v>
+        <v>-0.676</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>5.1411e-01</t>
+          <t>7.7742e-01</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1120,20 +1120,20 @@
         </is>
       </c>
       <c r="B23">
-        <v>-1.563</v>
+        <v>-1.464</v>
       </c>
       <c r="C23">
-        <v>0.589</v>
+        <v>0.541</v>
       </c>
       <c r="D23">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E23">
-        <v>-2.654</v>
+        <v>-2.705</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2.1890e-02</t>
+          <t>1.8855e-02</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1154,20 +1154,20 @@
         </is>
       </c>
       <c r="B24">
-        <v>-5.64</v>
+        <v>-4.295</v>
       </c>
       <c r="C24">
-        <v>1.425</v>
+        <v>1.345</v>
       </c>
       <c r="D24">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E24">
-        <v>-3.957</v>
+        <v>-3.194</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2.3296e-04</t>
+          <t>4.0689e-03</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1188,25 +1188,25 @@
         </is>
       </c>
       <c r="B25">
-        <v>-4.076</v>
+        <v>-2.831</v>
       </c>
       <c r="C25">
-        <v>1.43</v>
+        <v>1.349</v>
       </c>
       <c r="D25">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E25">
-        <v>-2.851</v>
+        <v>-2.098</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>1.2277e-02</t>
+          <t>9.0424e-02</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1222,20 +1222,20 @@
         </is>
       </c>
       <c r="B26">
-        <v>-0.8179999999999999</v>
+        <v>-0.796</v>
       </c>
       <c r="C26">
-        <v>0.292</v>
+        <v>0.267</v>
       </c>
       <c r="D26">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E26">
-        <v>-2.803</v>
+        <v>-2.98</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>1.4161e-02</t>
+          <t>8.1969e-03</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1256,20 +1256,20 @@
         </is>
       </c>
       <c r="B27">
-        <v>-2.02</v>
+        <v>-1.974</v>
       </c>
       <c r="C27">
-        <v>0.706</v>
+        <v>0.664</v>
       </c>
       <c r="D27">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E27">
-        <v>-2.861</v>
+        <v>-2.974</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>1.1912e-02</t>
+          <t>8.3491e-03</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1290,20 +1290,20 @@
         </is>
       </c>
       <c r="B28">
-        <v>-1.202</v>
+        <v>-1.178</v>
       </c>
       <c r="C28">
-        <v>0.708</v>
+        <v>0.666</v>
       </c>
       <c r="D28">
-        <v>1669</v>
+        <v>2007</v>
       </c>
       <c r="E28">
-        <v>-1.696</v>
+        <v>-1.769</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2.0694e-01</t>
+          <t>1.8025e-01</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">

</xml_diff>